<commit_message>
Run full test and test of the file gitignore
</commit_message>
<xml_diff>
--- a/DataConfig/TestData.xlsx
+++ b/DataConfig/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="25">
   <si>
     <t xml:space="preserve">URLHome</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>69.99</t>
+  </si>
+  <si>
+    <t>49.99</t>
+  </si>
+  <si>
+    <t>51.99</t>
+  </si>
+  <si>
+    <t>26.90</t>
   </si>
 </sst>
 </file>
@@ -329,13 +338,13 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>

</xml_diff>